<commit_message>
Feature Vectorization update for Badge dataset and User dataset
</commit_message>
<xml_diff>
--- a/data/user_dataset_updated.xlsx
+++ b/data/user_dataset_updated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Badgelens\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coolc\Documents\BadgeLens\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231BD778-7860-4C1C-A2EF-51B9FE0FBB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD60CA55-35C3-49A0-8368-56435CE7235E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,9 +361,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -401,9 +401,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,9 +436,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,9 +488,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -650,16 +684,20 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="8" max="8" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="14.69921875" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="7" width="34.3984375" customWidth="1"/>
+    <col min="8" max="8" width="18.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,7 +723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -711,7 +749,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -737,7 +775,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -763,7 +801,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -789,7 +827,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -815,7 +853,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -841,7 +879,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -867,7 +905,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -893,7 +931,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -919,7 +957,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>16</v>
       </c>

</xml_diff>